<commit_message>
everything works, cleaned code, added error checks, misc stuff
</commit_message>
<xml_diff>
--- a/dictionary.xlsx
+++ b/dictionary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,37 +449,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>simulator</t>
+          <t>meandering</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>One who simulates or feigns.;A machine or system that simulates an environment (such as an aircraft cockpit), often for training purposes.</t>
+          <t>To wind or turn in a course or passage; to be intricate.;To wind, turn, or twist; to make flexuous.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>симулятор</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>faint</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>The act of fainting, syncope.;The state of one who has fainted; a swoon.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>слабый</t>
+          <t>блуждающий</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added comments, cleaned code a bit
</commit_message>
<xml_diff>
--- a/dictionary.xlsx
+++ b/dictionary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,6 +463,26 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>lamenting</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>To express grief; to weep or wail; to mourn.;To feel great sorrow or regret; to bewail.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>оплакивать</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>